<commit_message>
Period highlight. README update. Empty cell will not be considered as any of the emotion types now."
</commit_message>
<xml_diff>
--- a/emotion_record_statistics/emotion_record.xlsx
+++ b/emotion_record_statistics/emotion_record.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\tools-programs\emotion_record_statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D532ADFD-4275-44B1-BAB2-48AB22D71A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BBB2A8-5F2C-4F45-B616-370AE019B14F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C852AB77-5F89-44F3-A590-1A1628580EA8}"/>
   </bookViews>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Numb</t>
   </si>
@@ -122,12 +116,6 @@
     <t>Chilling out</t>
   </si>
   <si>
-    <t>漏填的格子用最近的颜色填上
-长时间漏填留空白
-TODO:
-制作读取本表格的工具</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">I - </t>
     </r>
@@ -159,6 +147,70 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>漏填的格子用最近的颜色填上
+长时间漏填留空白</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Academic</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">E - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entertainments</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">R - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rapid emotion fluctuation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Integer - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Number of repetition</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -472,7 +524,7 @@
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -514,6 +566,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="8" fillId="14" borderId="1" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -550,12 +608,7 @@
     <xf numFmtId="0" fontId="10" fillId="16" borderId="1" xfId="15" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="14" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="14"/>
   </cellXfs>
   <cellStyles count="16">
     <cellStyle name="20% - 着色 6" xfId="12" builtinId="50"/>
@@ -888,7 +941,7 @@
   <dimension ref="A1:BD70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:D27"/>
+      <selection activeCell="AJ23" sqref="AI23:AJ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.33203125" defaultRowHeight="21.6" customHeight="1"/>
@@ -898,12 +951,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="21.6" customHeight="1">
-      <c r="A1" s="49" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="A1" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="6">
         <v>0.29166666666666669</v>
       </c>
@@ -1044,12 +1097,12 @@
       <c r="AJ2" s="32"/>
     </row>
     <row r="3" spans="1:56" ht="21.6" customHeight="1">
-      <c r="A3" s="50">
+      <c r="A3" s="37">
         <v>43938</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="27"/>
       <c r="F3" s="32"/>
       <c r="G3" s="34"/>
@@ -1082,6 +1135,7 @@
       <c r="AH3" s="30"/>
       <c r="AI3" s="32"/>
       <c r="AJ3" s="30"/>
+      <c r="AK3" s="51"/>
     </row>
     <row r="4" spans="1:56" ht="21.6" customHeight="1">
       <c r="A4" s="35">
@@ -1122,6 +1176,7 @@
       <c r="AH4" s="30"/>
       <c r="AI4" s="32"/>
       <c r="AJ4" s="30"/>
+      <c r="AK4" s="51"/>
     </row>
     <row r="5" spans="1:56" ht="21.6" customHeight="1">
       <c r="A5" s="35">
@@ -1162,22 +1217,23 @@
       <c r="AH5" s="30"/>
       <c r="AI5" s="32"/>
       <c r="AJ5" s="30"/>
-      <c r="AQ5" s="39" t="s">
+      <c r="AK5" s="51"/>
+      <c r="AQ5" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="AR5" s="40"/>
-      <c r="AS5" s="40"/>
-      <c r="AT5" s="40"/>
-      <c r="AU5" s="40"/>
-      <c r="AV5" s="40"/>
-      <c r="AW5" s="40"/>
-      <c r="AX5" s="40"/>
-      <c r="AY5" s="40"/>
-      <c r="AZ5" s="40"/>
-      <c r="BA5" s="40"/>
-      <c r="BB5" s="40"/>
-      <c r="BC5" s="40"/>
-      <c r="BD5" s="41"/>
+      <c r="AR5" s="42"/>
+      <c r="AS5" s="42"/>
+      <c r="AT5" s="42"/>
+      <c r="AU5" s="42"/>
+      <c r="AV5" s="42"/>
+      <c r="AW5" s="42"/>
+      <c r="AX5" s="42"/>
+      <c r="AY5" s="42"/>
+      <c r="AZ5" s="42"/>
+      <c r="BA5" s="42"/>
+      <c r="BB5" s="42"/>
+      <c r="BC5" s="42"/>
+      <c r="BD5" s="43"/>
     </row>
     <row r="6" spans="1:56" ht="21.6" customHeight="1">
       <c r="A6" s="35">
@@ -1218,11 +1274,12 @@
       <c r="AH6" s="30"/>
       <c r="AI6" s="32"/>
       <c r="AJ6" s="30"/>
-      <c r="AL6" s="45" t="s">
+      <c r="AK6" s="51"/>
+      <c r="AL6" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="AM6" s="45"/>
-      <c r="AN6" s="45"/>
+      <c r="AM6" s="47"/>
+      <c r="AN6" s="47"/>
       <c r="AQ6" s="19"/>
       <c r="AR6" s="2"/>
       <c r="AS6" s="2"/>
@@ -1277,11 +1334,12 @@
       <c r="AH7" s="30"/>
       <c r="AI7" s="32"/>
       <c r="AJ7" s="30"/>
-      <c r="AL7" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="AM7" s="46"/>
-      <c r="AN7" s="46"/>
+      <c r="AK7" s="51"/>
+      <c r="AL7" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM7" s="48"/>
+      <c r="AN7" s="48"/>
       <c r="AQ7" s="20"/>
       <c r="AR7" s="16" t="s">
         <v>0</v>
@@ -1339,9 +1397,10 @@
       <c r="AH8" s="30"/>
       <c r="AI8" s="32"/>
       <c r="AJ8" s="30"/>
-      <c r="AL8" s="46"/>
-      <c r="AM8" s="46"/>
-      <c r="AN8" s="46"/>
+      <c r="AK8" s="51"/>
+      <c r="AL8" s="48"/>
+      <c r="AM8" s="48"/>
+      <c r="AN8" s="48"/>
       <c r="AQ8" s="19"/>
       <c r="AR8" s="2"/>
       <c r="AS8" s="2"/>
@@ -1398,9 +1457,9 @@
       <c r="AH9" s="30"/>
       <c r="AI9" s="32"/>
       <c r="AJ9" s="30"/>
-      <c r="AL9" s="46"/>
-      <c r="AM9" s="46"/>
-      <c r="AN9" s="46"/>
+      <c r="AL9" s="48"/>
+      <c r="AM9" s="48"/>
+      <c r="AN9" s="48"/>
       <c r="AP9" s="3"/>
       <c r="AQ9" s="11"/>
       <c r="AR9" s="16" t="s">
@@ -1416,7 +1475,7 @@
       <c r="AX9" s="2"/>
       <c r="AY9" s="3"/>
       <c r="AZ9" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="BA9" s="2"/>
       <c r="BB9" s="2"/>
@@ -1462,9 +1521,9 @@
       <c r="AH10" s="30"/>
       <c r="AI10" s="32"/>
       <c r="AJ10" s="30"/>
-      <c r="AL10" s="46"/>
-      <c r="AM10" s="46"/>
-      <c r="AN10" s="46"/>
+      <c r="AL10" s="48"/>
+      <c r="AM10" s="48"/>
+      <c r="AN10" s="48"/>
       <c r="AP10" s="3"/>
       <c r="AQ10" s="12"/>
       <c r="AR10" s="16" t="s">
@@ -1482,7 +1541,7 @@
       </c>
       <c r="AY10" s="3"/>
       <c r="AZ10" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BA10" s="2"/>
       <c r="BB10" s="17"/>
@@ -1528,9 +1587,9 @@
       <c r="AH11" s="30"/>
       <c r="AI11" s="32"/>
       <c r="AJ11" s="30"/>
-      <c r="AL11" s="46"/>
-      <c r="AM11" s="46"/>
-      <c r="AN11" s="46"/>
+      <c r="AL11" s="48"/>
+      <c r="AM11" s="48"/>
+      <c r="AN11" s="48"/>
       <c r="AP11" s="3"/>
       <c r="AQ11" s="13"/>
       <c r="AR11" s="16" t="s">
@@ -1547,7 +1606,9 @@
         <v>3</v>
       </c>
       <c r="AY11" s="3"/>
-      <c r="AZ11" s="19"/>
+      <c r="AZ11" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="BA11" s="2"/>
       <c r="BB11" s="2"/>
       <c r="BC11" s="2"/>
@@ -1592,9 +1653,9 @@
       <c r="AH12" s="30"/>
       <c r="AI12" s="32"/>
       <c r="AJ12" s="30"/>
-      <c r="AL12" s="46"/>
-      <c r="AM12" s="46"/>
-      <c r="AN12" s="46"/>
+      <c r="AL12" s="48"/>
+      <c r="AM12" s="48"/>
+      <c r="AN12" s="48"/>
       <c r="AP12" s="3"/>
       <c r="AQ12" s="14"/>
       <c r="AR12" s="16" t="s">
@@ -1609,7 +1670,9 @@
       <c r="AW12" s="2"/>
       <c r="AX12" s="2"/>
       <c r="AY12" s="3"/>
-      <c r="AZ12" s="19"/>
+      <c r="AZ12" s="24" t="s">
+        <v>24</v>
+      </c>
       <c r="BA12" s="2"/>
       <c r="BB12" s="2"/>
       <c r="BC12" s="2"/>
@@ -1654,9 +1717,9 @@
       <c r="AH13" s="30"/>
       <c r="AI13" s="32"/>
       <c r="AJ13" s="30"/>
-      <c r="AL13" s="46"/>
-      <c r="AM13" s="46"/>
-      <c r="AN13" s="46"/>
+      <c r="AL13" s="48"/>
+      <c r="AM13" s="48"/>
+      <c r="AN13" s="48"/>
       <c r="AP13" s="3"/>
       <c r="AQ13" s="2"/>
       <c r="AR13" s="2"/>
@@ -1667,7 +1730,9 @@
       <c r="AW13" s="2"/>
       <c r="AX13" s="2"/>
       <c r="AY13" s="3"/>
-      <c r="AZ13" s="19"/>
+      <c r="AZ13" s="24" t="s">
+        <v>25</v>
+      </c>
       <c r="BA13" s="2"/>
       <c r="BB13" s="2"/>
       <c r="BC13" s="2"/>
@@ -1712,12 +1777,14 @@
       <c r="AH14" s="30"/>
       <c r="AI14" s="32"/>
       <c r="AJ14" s="30"/>
-      <c r="AL14" s="46"/>
-      <c r="AM14" s="46"/>
-      <c r="AN14" s="46"/>
+      <c r="AL14" s="48"/>
+      <c r="AM14" s="48"/>
+      <c r="AN14" s="48"/>
       <c r="AP14" s="3"/>
       <c r="AY14" s="3"/>
-      <c r="AZ14" s="19"/>
+      <c r="AZ14" s="24" t="s">
+        <v>26</v>
+      </c>
       <c r="BA14" s="2"/>
       <c r="BB14" s="2"/>
       <c r="BC14" s="2"/>
@@ -1810,34 +1877,34 @@
       <c r="AI16" s="32"/>
       <c r="AJ16" s="30"/>
       <c r="AP16" s="3"/>
-      <c r="AQ16" s="42" t="s">
+      <c r="AQ16" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="AR16" s="43"/>
-      <c r="AS16" s="43"/>
-      <c r="AT16" s="43" t="s">
+      <c r="AR16" s="45"/>
+      <c r="AS16" s="45"/>
+      <c r="AT16" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="AU16" s="43"/>
-      <c r="AV16" s="43"/>
-      <c r="AW16" s="43" t="s">
+      <c r="AU16" s="45"/>
+      <c r="AV16" s="45"/>
+      <c r="AW16" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="AX16" s="43"/>
-      <c r="AY16" s="44"/>
+      <c r="AX16" s="45"/>
+      <c r="AY16" s="46"/>
       <c r="AZ16" s="21"/>
       <c r="BA16" s="4"/>
       <c r="BB16" s="4"/>
       <c r="BC16" s="4"/>
       <c r="BD16" s="5"/>
     </row>
-    <row r="17" spans="1:36" ht="21.6" customHeight="1">
-      <c r="A17" s="37">
+    <row r="17" spans="1:37" ht="21.6" customHeight="1">
+      <c r="A17" s="39">
         <v>43952</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
       <c r="E17" s="27"/>
       <c r="F17" s="32"/>
       <c r="G17" s="34"/>
@@ -1871,7 +1938,7 @@
       <c r="AI17" s="32"/>
       <c r="AJ17" s="30"/>
     </row>
-    <row r="18" spans="1:36" ht="21.6" customHeight="1">
+    <row r="18" spans="1:37" ht="21.6" customHeight="1">
       <c r="A18" s="35">
         <v>43953</v>
       </c>
@@ -1911,7 +1978,7 @@
       <c r="AI18" s="32"/>
       <c r="AJ18" s="30"/>
     </row>
-    <row r="19" spans="1:36" ht="21.6" customHeight="1">
+    <row r="19" spans="1:37" ht="21.6" customHeight="1">
       <c r="A19" s="35">
         <v>43954</v>
       </c>
@@ -1951,7 +2018,7 @@
       <c r="AI19" s="32"/>
       <c r="AJ19" s="30"/>
     </row>
-    <row r="20" spans="1:36" ht="21.6" customHeight="1">
+    <row r="20" spans="1:37" ht="21.6" customHeight="1">
       <c r="A20" s="35">
         <v>43955</v>
       </c>
@@ -1991,7 +2058,7 @@
       <c r="AI20" s="32"/>
       <c r="AJ20" s="30"/>
     </row>
-    <row r="21" spans="1:36" ht="21.6" customHeight="1">
+    <row r="21" spans="1:37" ht="21.6" customHeight="1">
       <c r="A21" s="35">
         <v>43956</v>
       </c>
@@ -2031,7 +2098,7 @@
       <c r="AI21" s="32"/>
       <c r="AJ21" s="30"/>
     </row>
-    <row r="22" spans="1:36" ht="21.6" customHeight="1">
+    <row r="22" spans="1:37" ht="21.6" customHeight="1">
       <c r="A22" s="35">
         <v>43957</v>
       </c>
@@ -2071,7 +2138,7 @@
       <c r="AI22" s="32"/>
       <c r="AJ22" s="30"/>
     </row>
-    <row r="23" spans="1:36" ht="21.6" customHeight="1">
+    <row r="23" spans="1:37" ht="21.6" customHeight="1">
       <c r="A23" s="35">
         <v>43958</v>
       </c>
@@ -2111,7 +2178,7 @@
       <c r="AI23" s="32"/>
       <c r="AJ23" s="30"/>
     </row>
-    <row r="24" spans="1:36" ht="21.6" customHeight="1">
+    <row r="24" spans="1:37" ht="21.6" customHeight="1">
       <c r="A24" s="35">
         <v>43959</v>
       </c>
@@ -2151,7 +2218,7 @@
       <c r="AI24" s="32"/>
       <c r="AJ24" s="30"/>
     </row>
-    <row r="25" spans="1:36" ht="21.6" customHeight="1">
+    <row r="25" spans="1:37" ht="21.6" customHeight="1">
       <c r="A25" s="35">
         <v>43960</v>
       </c>
@@ -2191,7 +2258,7 @@
       <c r="AI25" s="32"/>
       <c r="AJ25" s="30"/>
     </row>
-    <row r="26" spans="1:36" ht="21.6" customHeight="1">
+    <row r="26" spans="1:37" ht="21.6" customHeight="1">
       <c r="A26" s="35">
         <v>43961</v>
       </c>
@@ -2231,13 +2298,13 @@
       <c r="AI26" s="32"/>
       <c r="AJ26" s="30"/>
     </row>
-    <row r="27" spans="1:36" ht="21.6" customHeight="1">
-      <c r="A27" s="47">
+    <row r="27" spans="1:37" ht="21.6" customHeight="1">
+      <c r="A27" s="49">
         <v>43962</v>
       </c>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
       <c r="E27" s="27"/>
       <c r="F27" s="32"/>
       <c r="G27" s="34"/>
@@ -2271,7 +2338,7 @@
       <c r="AI27" s="32"/>
       <c r="AJ27" s="30"/>
     </row>
-    <row r="28" spans="1:36" ht="21.6" customHeight="1">
+    <row r="28" spans="1:37" ht="21.6" customHeight="1">
       <c r="A28" s="35">
         <v>43963</v>
       </c>
@@ -2311,7 +2378,7 @@
       <c r="AI28" s="7"/>
       <c r="AJ28" s="7"/>
     </row>
-    <row r="29" spans="1:36" ht="21.6" customHeight="1">
+    <row r="29" spans="1:37" ht="21.6" customHeight="1">
       <c r="A29" s="35">
         <v>43964</v>
       </c>
@@ -2350,8 +2417,9 @@
       <c r="AH29" s="7"/>
       <c r="AI29" s="7"/>
       <c r="AJ29" s="7"/>
-    </row>
-    <row r="30" spans="1:36" ht="21.6" customHeight="1">
+      <c r="AK29" s="51"/>
+    </row>
+    <row r="30" spans="1:37" ht="21.6" customHeight="1">
       <c r="A30" s="35">
         <v>43965</v>
       </c>
@@ -2390,8 +2458,9 @@
       <c r="AH30" s="7"/>
       <c r="AI30" s="7"/>
       <c r="AJ30" s="7"/>
-    </row>
-    <row r="31" spans="1:36" ht="21.6" customHeight="1">
+      <c r="AK30" s="51"/>
+    </row>
+    <row r="31" spans="1:37" ht="21.6" customHeight="1">
       <c r="A31" s="35">
         <v>43966</v>
       </c>
@@ -2430,8 +2499,9 @@
       <c r="AH31" s="7"/>
       <c r="AI31" s="7"/>
       <c r="AJ31" s="7"/>
-    </row>
-    <row r="32" spans="1:36" ht="21.6" customHeight="1">
+      <c r="AK31" s="51"/>
+    </row>
+    <row r="32" spans="1:37" ht="21.6" customHeight="1">
       <c r="A32" s="35">
         <v>43967</v>
       </c>
@@ -2470,8 +2540,9 @@
       <c r="AH32" s="7"/>
       <c r="AI32" s="7"/>
       <c r="AJ32" s="7"/>
-    </row>
-    <row r="33" spans="1:36" ht="21.6" customHeight="1">
+      <c r="AK32" s="51"/>
+    </row>
+    <row r="33" spans="1:37" ht="21.6" customHeight="1">
       <c r="A33" s="35">
         <v>43968</v>
       </c>
@@ -2510,8 +2581,9 @@
       <c r="AH33" s="7"/>
       <c r="AI33" s="7"/>
       <c r="AJ33" s="7"/>
-    </row>
-    <row r="34" spans="1:36" ht="21.6" customHeight="1">
+      <c r="AK33" s="51"/>
+    </row>
+    <row r="34" spans="1:37" ht="21.6" customHeight="1">
       <c r="A34" s="35">
         <v>43969</v>
       </c>
@@ -2550,8 +2622,9 @@
       <c r="AH34" s="7"/>
       <c r="AI34" s="7"/>
       <c r="AJ34" s="7"/>
-    </row>
-    <row r="35" spans="1:36" ht="21.6" customHeight="1">
+      <c r="AK34" s="51"/>
+    </row>
+    <row r="35" spans="1:37" ht="21.6" customHeight="1">
       <c r="A35" s="35">
         <v>43970</v>
       </c>
@@ -2591,7 +2664,7 @@
       <c r="AI35" s="7"/>
       <c r="AJ35" s="7"/>
     </row>
-    <row r="36" spans="1:36" ht="21.6" customHeight="1">
+    <row r="36" spans="1:37" ht="21.6" customHeight="1">
       <c r="A36" s="35">
         <v>43971</v>
       </c>
@@ -2631,7 +2704,7 @@
       <c r="AI36" s="7"/>
       <c r="AJ36" s="7"/>
     </row>
-    <row r="37" spans="1:36" ht="21.6" customHeight="1">
+    <row r="37" spans="1:37" ht="21.6" customHeight="1">
       <c r="A37" s="35">
         <v>43972</v>
       </c>
@@ -2671,7 +2744,7 @@
       <c r="AI37" s="7"/>
       <c r="AJ37" s="7"/>
     </row>
-    <row r="38" spans="1:36" ht="21.6" customHeight="1">
+    <row r="38" spans="1:37" ht="21.6" customHeight="1">
       <c r="A38" s="35">
         <v>43973</v>
       </c>
@@ -2711,7 +2784,7 @@
       <c r="AI38" s="7"/>
       <c r="AJ38" s="7"/>
     </row>
-    <row r="39" spans="1:36" ht="21.6" customHeight="1">
+    <row r="39" spans="1:37" ht="21.6" customHeight="1">
       <c r="A39" s="35">
         <v>43974</v>
       </c>
@@ -2751,7 +2824,7 @@
       <c r="AI39" s="7"/>
       <c r="AJ39" s="7"/>
     </row>
-    <row r="40" spans="1:36" ht="21.6" customHeight="1">
+    <row r="40" spans="1:37" ht="21.6" customHeight="1">
       <c r="A40" s="35">
         <v>43975</v>
       </c>
@@ -2791,7 +2864,7 @@
       <c r="AI40" s="7"/>
       <c r="AJ40" s="7"/>
     </row>
-    <row r="41" spans="1:36" ht="21.6" customHeight="1">
+    <row r="41" spans="1:37" ht="21.6" customHeight="1">
       <c r="A41" s="35">
         <v>43976</v>
       </c>
@@ -2831,7 +2904,7 @@
       <c r="AI41" s="7"/>
       <c r="AJ41" s="7"/>
     </row>
-    <row r="42" spans="1:36" ht="21.6" customHeight="1">
+    <row r="42" spans="1:37" ht="21.6" customHeight="1">
       <c r="A42" s="35">
         <v>43977</v>
       </c>
@@ -2871,7 +2944,7 @@
       <c r="AI42" s="7"/>
       <c r="AJ42" s="7"/>
     </row>
-    <row r="43" spans="1:36" ht="21.6" customHeight="1">
+    <row r="43" spans="1:37" ht="21.6" customHeight="1">
       <c r="A43" s="35">
         <v>43978</v>
       </c>
@@ -2911,7 +2984,7 @@
       <c r="AI43" s="7"/>
       <c r="AJ43" s="7"/>
     </row>
-    <row r="44" spans="1:36" ht="21.6" customHeight="1">
+    <row r="44" spans="1:37" ht="21.6" customHeight="1">
       <c r="A44" s="35">
         <v>43979</v>
       </c>
@@ -2951,7 +3024,7 @@
       <c r="AI44" s="7"/>
       <c r="AJ44" s="7"/>
     </row>
-    <row r="45" spans="1:36" ht="21.6" customHeight="1">
+    <row r="45" spans="1:37" ht="21.6" customHeight="1">
       <c r="A45" s="35">
         <v>43980</v>
       </c>
@@ -2991,7 +3064,7 @@
       <c r="AI45" s="7"/>
       <c r="AJ45" s="7"/>
     </row>
-    <row r="46" spans="1:36" ht="21.6" customHeight="1">
+    <row r="46" spans="1:37" ht="21.6" customHeight="1">
       <c r="A46" s="35">
         <v>43981</v>
       </c>
@@ -3031,7 +3104,7 @@
       <c r="AI46" s="7"/>
       <c r="AJ46" s="7"/>
     </row>
-    <row r="47" spans="1:36" ht="21.6" customHeight="1">
+    <row r="47" spans="1:37" ht="21.6" customHeight="1">
       <c r="A47" s="35">
         <v>43982</v>
       </c>
@@ -3071,13 +3144,13 @@
       <c r="AI47" s="7"/>
       <c r="AJ47" s="7"/>
     </row>
-    <row r="48" spans="1:36" ht="21.6" customHeight="1">
-      <c r="A48" s="37">
+    <row r="48" spans="1:37" ht="21.6" customHeight="1">
+      <c r="A48" s="39">
         <v>43983</v>
       </c>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
@@ -3993,26 +4066,46 @@
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A67:D67"/>
+    <mergeCell ref="A68:D68"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="AQ5:BD5"/>
     <mergeCell ref="AQ16:AS16"/>
@@ -4029,46 +4122,26 @@
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A57:D57"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A67:D67"/>
-    <mergeCell ref="A68:D68"/>
-    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>